<commit_message>
[Documentation] Setup of mapping
</commit_message>
<xml_diff>
--- a/Documentation/data mapping.xlsx
+++ b/Documentation/data mapping.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lu\Documents\git\OS4-Mario\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaker\Desktop\Dev\OS4-Mario\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24FA3ED4-4580-45E5-BE86-78A0811A5C5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C752554D-4245-4CFA-885E-3E131E2BD3C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="525" yWindow="435" windowWidth="23145" windowHeight="13185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="65">
   <si>
     <t>Pizzabodems bestand:</t>
   </si>
@@ -138,15 +138,6 @@
     <t>Aantal</t>
   </si>
   <si>
-    <t xml:space="preserve">Extra </t>
-  </si>
-  <si>
-    <t>IngrediÃ«nten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prijs </t>
-  </si>
-  <si>
     <t>Regelprijs</t>
   </si>
   <si>
@@ -166,6 +157,69 @@
   </si>
   <si>
     <t>Table</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>PropertyKey</t>
+  </si>
+  <si>
+    <t>PropertyValue</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>DeliverySurcharge</t>
+  </si>
+  <si>
+    <t>Restaurant</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>PlacementDate</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>DeliveryDate</t>
+  </si>
+  <si>
+    <t>ProductId</t>
+  </si>
+  <si>
+    <t>OrderItem</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>OrderItemProperty</t>
+  </si>
+  <si>
+    <t>note: OrderItemId van Product</t>
+  </si>
+  <si>
+    <t>CouponId</t>
+  </si>
+  <si>
+    <t>Extra-IngrediÃ«nten</t>
+  </si>
+  <si>
+    <t>Prijs-Extra-IngrediÃ«nten</t>
   </si>
 </sst>
 </file>
@@ -220,7 +274,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -498,19 +552,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5546875" customWidth="1"/>
-    <col min="2" max="2" width="17.77734375" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -518,269 +574,467 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C36" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C38" t="s">
+        <v>56</v>
+      </c>
+      <c r="D38" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C39" t="s">
+        <v>56</v>
+      </c>
+      <c r="D39" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C40" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C41" t="s">
+        <v>57</v>
+      </c>
+      <c r="D41" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C42" t="s">
+        <v>57</v>
+      </c>
+      <c r="D42" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C44" t="s">
+        <v>59</v>
+      </c>
+      <c r="D44" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C45" t="s">
+        <v>45</v>
+      </c>
+      <c r="D45" t="s">
+        <v>60</v>
+      </c>
+      <c r="E45" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>62</v>
+      </c>
+      <c r="D49" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Documentation] Fix table names
</commit_message>
<xml_diff>
--- a/Documentation/data mapping.xlsx
+++ b/Documentation/data mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaker\Desktop\Dev\OS4-Mario\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C752554D-4245-4CFA-885E-3E131E2BD3C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC4668E6-16C3-49BC-B66E-973CB5B8B963}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="525" yWindow="435" windowWidth="23145" windowHeight="13185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="66">
   <si>
     <t>Pizzabodems bestand:</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t>Prijs-Extra-IngrediÃ«nten</t>
+  </si>
+  <si>
+    <t>ProductProperty</t>
   </si>
 </sst>
 </file>
@@ -555,7 +558,7 @@
   <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,7 +711,7 @@
         <v>45</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -719,7 +722,7 @@
         <v>45</v>
       </c>
       <c r="D16" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -730,7 +733,7 @@
         <v>45</v>
       </c>
       <c r="D17" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -741,7 +744,7 @@
         <v>45</v>
       </c>
       <c r="D18" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -812,7 +815,7 @@
         <v>45</v>
       </c>
       <c r="D26" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -823,7 +826,7 @@
         <v>45</v>
       </c>
       <c r="D27" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>